<commit_message>
added support for messages
</commit_message>
<xml_diff>
--- a/test_data_RA.xlsx
+++ b/test_data_RA.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayushmanroy/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ayushmanroy/Desktop/Roommate_Matching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4F3877-D537-C942-AC95-67C42EAE8826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E40BC2E8-DB7C-C247-9CCB-F7CE5B1157D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="15780" xr2:uid="{F133B0AD-67AC-E84F-A673-BF772185E7F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>NAME</t>
   </si>
@@ -105,18 +105,51 @@
   </si>
   <si>
     <t>WEIGHTS</t>
+  </si>
+  <si>
+    <t>MESSAGES</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>ghi</t>
+  </si>
+  <si>
+    <t>jkl</t>
+  </si>
+  <si>
+    <t>mno</t>
+  </si>
+  <si>
+    <t>pqr</t>
+  </si>
+  <si>
+    <t>stv</t>
+  </si>
+  <si>
+    <t>wxy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="TimesNewRomanPSMT"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,8 +172,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05453D66-ECCB-7840-91FF-EEFBB42008A1}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="H1" sqref="H1:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -505,6 +539,9 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="J1" t="s">
         <v>22</v>
       </c>
@@ -534,6 +571,9 @@
         <f>$K$4*F2</f>
         <v>7.5</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="J2" t="s">
         <v>19</v>
       </c>
@@ -566,6 +606,9 @@
         <f t="shared" ref="G3:G13" si="2">$K$4*F3</f>
         <v>7.5</v>
       </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="J3" t="s">
         <v>20</v>
       </c>
@@ -598,6 +641,9 @@
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
+      <c r="H4" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="J4" t="s">
         <v>21</v>
       </c>
@@ -630,6 +676,9 @@
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" t="s">
@@ -656,6 +705,9 @@
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
+      <c r="H6" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="7" spans="1:11">
       <c r="A7" t="s">
@@ -682,6 +734,9 @@
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:11">
       <c r="A8" t="s">
@@ -708,6 +763,9 @@
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
+      <c r="H8" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="9" spans="1:11">
       <c r="A9" t="s">
@@ -734,6 +792,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="H9" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
@@ -760,6 +821,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" t="s">
@@ -786,6 +850,9 @@
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
@@ -812,6 +879,9 @@
         <f t="shared" si="2"/>
         <v>2.5</v>
       </c>
+      <c r="H12" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
@@ -838,6 +908,12 @@
         <f t="shared" si="2"/>
         <v>7.5</v>
       </c>
+      <c r="H13" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="H14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>